<commit_message>
Changed config files to operational settings and METADATA
- Config files were adapted to operational settings to test
  the respective script 'operational/script_run_operational.py'.
- Changed naming of METADATA variables (e.g. all capital letters)
</commit_message>
<xml_diff>
--- a/config/cfg_var.xlsx
+++ b/config/cfg_var.xlsx
@@ -613,7 +613,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="315">
   <si>
     <t>VARIABLE</t>
   </si>
@@ -822,9 +822,6 @@
     <t>SOLAR_TIME_COS</t>
   </si>
   <si>
-    <t>TOPOGRAPHY</t>
-  </si>
-  <si>
     <t>COSMO_CONV</t>
   </si>
   <si>
@@ -1545,7 +1542,22 @@
     <t>Slope</t>
   </si>
   <si>
-    <t>Aspect</t>
+    <t>TOPO_ASPECT</t>
+  </si>
+  <si>
+    <t>TOPO_ALTITUDE</t>
+  </si>
+  <si>
+    <t>TOPO_SLOPE</t>
+  </si>
+  <si>
+    <t>RADAR_FREQ_QUAL</t>
+  </si>
+  <si>
+    <t>Radar quality index</t>
+  </si>
+  <si>
+    <t>Dot product of U/V_OFLOW vector and Aspect vector</t>
   </si>
 </sst>
 </file>
@@ -2277,7 +2289,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="210">
+  <dxfs count="214">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4675,11 +4727,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF97"/>
+  <dimension ref="A1:AF98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L92" sqref="L92"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4699,28 +4751,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>295</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="57" t="s">
-        <v>296</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>300</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>66</v>
@@ -4732,13 +4784,13 @@
         <v>3</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>4</v>
@@ -4750,25 +4802,25 @@
         <v>6</v>
       </c>
       <c r="S1" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="W1" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>242</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>243</v>
       </c>
       <c r="Z1" s="4" t="s">
         <v>7</v>
@@ -4777,13 +4829,13 @@
         <v>27</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -4791,16 +4843,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" s="45">
         <v>0.05</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F2" s="45">
         <v>0</v>
@@ -4881,19 +4933,19 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" s="38">
         <v>0</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F3" s="45">
         <v>0</v>
@@ -4977,16 +5029,16 @@
         <v>9</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="38">
         <v>0.5</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F4" s="45">
         <v>0</v>
@@ -5070,16 +5122,16 @@
         <v>10</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="38">
         <v>0</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F5" s="45">
         <v>0</v>
@@ -5161,19 +5213,19 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="38">
         <v>0</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F6" s="45">
         <v>0</v>
@@ -5255,19 +5307,19 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="38">
         <v>0</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F7" s="45">
         <v>0</v>
@@ -5348,19 +5400,19 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="38">
         <v>0</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F8" s="45">
         <v>0</v>
@@ -5441,19 +5493,19 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="38">
         <v>0</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F9" s="45">
         <v>0</v>
@@ -5537,16 +5589,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="38">
         <v>-32</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F10" s="45">
         <v>0</v>
@@ -5630,16 +5682,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" s="49">
         <v>0</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F11" s="49">
         <v>0</v>
@@ -5723,16 +5775,16 @@
         <v>13</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C12" s="46">
         <v>0</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F12" s="47">
         <v>0</v>
@@ -5816,16 +5868,16 @@
         <v>14</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C13" s="47">
         <v>0</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F13" s="47">
         <v>0</v>
@@ -5909,16 +5961,16 @@
         <v>18</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C14" s="47">
         <v>0</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F14" s="47">
         <v>0</v>
@@ -6002,16 +6054,16 @@
         <v>17</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C15" s="47">
         <v>0</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F15" s="47">
         <v>0</v>
@@ -6095,16 +6147,16 @@
         <v>26</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C16" s="47">
         <v>0</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F16" s="47">
         <v>0</v>
@@ -6188,16 +6240,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C17" s="47">
         <v>0</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F17" s="47">
         <v>0</v>
@@ -6281,16 +6333,16 @@
         <v>15</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C18" s="47">
         <v>0</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F18" s="47">
         <v>0</v>
@@ -6374,16 +6426,16 @@
         <v>19</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C19" s="47">
         <v>0</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F19" s="47">
         <v>0</v>
@@ -6467,16 +6519,16 @@
         <v>20</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C20" s="47">
         <v>0</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F20" s="47">
         <v>0</v>
@@ -6560,16 +6612,16 @@
         <v>22</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C21" s="47">
         <v>0</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F21" s="47">
         <v>0</v>
@@ -6653,16 +6705,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C22" s="47">
         <v>0</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F22" s="47">
         <v>0</v>
@@ -6746,16 +6798,16 @@
         <v>23</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C23" s="47">
         <v>0</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F23" s="47">
         <v>0</v>
@@ -6836,25 +6888,25 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F24" s="37">
         <v>4</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H24" s="22">
         <v>0</v>
@@ -6929,25 +6981,25 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C25" s="45" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F25" s="38">
         <v>15</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H25" s="12">
         <v>0</v>
@@ -7022,25 +7074,25 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="C26" s="45" t="s">
+        <v>296</v>
+      </c>
+      <c r="D26" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="C26" s="45" t="s">
-        <v>297</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>137</v>
-      </c>
       <c r="E26" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F26" s="48">
         <v>0</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H26" s="12">
         <v>0</v>
@@ -7115,25 +7167,25 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F27" s="48">
         <v>0</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H27" s="12">
         <v>0</v>
@@ -7208,25 +7260,25 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C28" s="45" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F28" s="48">
         <v>0</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H28" s="25">
         <v>0</v>
@@ -7304,28 +7356,28 @@
         <v>29</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C29" s="46">
         <v>-180</v>
       </c>
       <c r="D29" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="E29" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="E29" s="26" t="s">
-        <v>256</v>
-      </c>
       <c r="F29" s="46">
         <v>0</v>
       </c>
       <c r="G29" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H29" s="22">
         <v>1</v>
       </c>
       <c r="I29" s="7">
-        <f t="shared" si="0"/>
+        <f>IF(OR(J29=1,I91=1),1,H29)</f>
         <v>1</v>
       </c>
       <c r="J29" s="22">
@@ -7397,28 +7449,28 @@
         <v>30</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C30" s="47">
         <v>-90</v>
       </c>
       <c r="D30" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="E30" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="E30" s="14" t="s">
-        <v>256</v>
-      </c>
       <c r="F30" s="47">
         <v>0</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H30" s="12">
         <v>1</v>
       </c>
       <c r="I30" s="7">
-        <f t="shared" si="0"/>
+        <f>IF(OR(J30=1,I91=1),1,H30)</f>
         <v>1</v>
       </c>
       <c r="J30" s="12">
@@ -7490,22 +7542,22 @@
         <v>31</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C31" s="47">
         <v>0</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F31" s="47">
         <v>0</v>
       </c>
       <c r="G31" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H31" s="12">
         <v>1</v>
@@ -7583,22 +7635,22 @@
         <v>32</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F32" s="47">
         <v>0</v>
       </c>
       <c r="G32" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H32" s="12">
         <v>1</v>
@@ -7676,22 +7728,22 @@
         <v>33</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C33" s="47">
         <v>0</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F33" s="47">
         <v>0</v>
       </c>
       <c r="G33" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H33" s="12">
         <v>1</v>
@@ -7769,22 +7821,22 @@
         <v>34</v>
       </c>
       <c r="B34" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="47">
+        <v>0</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C34" s="47">
-        <v>0</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>167</v>
-      </c>
       <c r="E34" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F34" s="47">
         <v>0</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H34" s="12">
         <v>1</v>
@@ -7862,22 +7914,22 @@
         <v>35</v>
       </c>
       <c r="B35" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C35" s="47">
+        <v>0</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C35" s="47">
-        <v>0</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>169</v>
-      </c>
       <c r="E35" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F35" s="47">
         <v>0</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H35" s="12">
         <v>1</v>
@@ -7955,22 +8007,22 @@
         <v>36</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C36" s="47">
         <v>0</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F36" s="47">
         <v>0</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H36" s="12">
         <v>1</v>
@@ -8048,22 +8100,22 @@
         <v>37</v>
       </c>
       <c r="B37" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C37" s="47">
+        <v>0</v>
+      </c>
+      <c r="D37" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="C37" s="47">
-        <v>0</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>173</v>
-      </c>
       <c r="E37" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F37" s="47">
         <v>0</v>
       </c>
       <c r="G37" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H37" s="12">
         <v>1</v>
@@ -8141,22 +8193,22 @@
         <v>38</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" s="47">
         <v>0</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F38" s="47">
         <v>0</v>
       </c>
       <c r="G38" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H38" s="12">
         <v>1</v>
@@ -8234,22 +8286,22 @@
         <v>39</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" s="47">
         <v>0</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F39" s="47">
         <v>0</v>
       </c>
       <c r="G39" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H39" s="12">
         <v>1</v>
@@ -8327,22 +8379,22 @@
         <v>40</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C40" s="47">
         <v>0</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F40" s="47">
         <v>0</v>
       </c>
       <c r="G40" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H40" s="12">
         <v>1</v>
@@ -8420,22 +8472,22 @@
         <v>41</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C41" s="47">
         <v>0</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F41" s="47">
         <v>0</v>
       </c>
       <c r="G41" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H41" s="12">
         <v>1</v>
@@ -8513,22 +8565,22 @@
         <v>42</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C42" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F42" s="47">
         <v>0</v>
       </c>
       <c r="G42" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H42" s="12">
         <v>1</v>
@@ -8606,22 +8658,22 @@
         <v>43</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C43" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F43" s="47">
         <v>0</v>
       </c>
       <c r="G43" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H43" s="12">
         <v>1</v>
@@ -8696,25 +8748,25 @@
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C44" s="47">
         <v>0</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F44" s="47">
         <v>0</v>
       </c>
       <c r="G44" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H44" s="12">
         <v>1</v>
@@ -8792,22 +8844,22 @@
         <v>44</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C45" s="47">
         <v>0</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F45" s="47">
         <v>0</v>
       </c>
       <c r="G45" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H45" s="12">
         <v>1</v>
@@ -8885,22 +8937,22 @@
         <v>45</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C46" s="47">
         <v>0</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F46" s="47">
         <v>0</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H46" s="12">
         <v>1</v>
@@ -8978,22 +9030,22 @@
         <v>46</v>
       </c>
       <c r="B47" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C47" s="47">
+        <v>0</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="C47" s="47">
-        <v>0</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>184</v>
-      </c>
       <c r="E47" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F47" s="47">
         <v>0</v>
       </c>
       <c r="G47" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H47" s="12">
         <v>1</v>
@@ -9071,22 +9123,22 @@
         <v>47</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C48" s="47">
         <v>0</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F48" s="47">
         <v>0</v>
       </c>
       <c r="G48" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H48" s="12">
         <v>1</v>
@@ -9164,22 +9216,22 @@
         <v>50</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C49" s="47">
         <v>0</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F49" s="47">
         <v>0</v>
       </c>
       <c r="G49" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H49" s="12">
         <v>1</v>
@@ -9257,22 +9309,22 @@
         <v>51</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C50" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F50" s="47">
         <v>0</v>
       </c>
       <c r="G50" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H50" s="12">
         <v>1</v>
@@ -9350,22 +9402,22 @@
         <v>52</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C51" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F51" s="47">
         <v>0</v>
       </c>
       <c r="G51" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H51" s="12">
         <v>1</v>
@@ -9440,25 +9492,25 @@
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C52" s="47">
         <v>0</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F52" s="47">
         <v>0</v>
       </c>
       <c r="G52" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H52" s="12">
         <v>1</v>
@@ -9533,25 +9585,25 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C53" s="47">
         <v>0</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F53" s="47">
         <v>0</v>
       </c>
       <c r="G53" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H53" s="12">
         <v>1</v>
@@ -9629,22 +9681,22 @@
         <v>53</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C54" s="58">
         <v>0</v>
       </c>
       <c r="D54" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F54" s="47">
         <v>0</v>
       </c>
       <c r="G54" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H54" s="12">
         <v>0</v>
@@ -9722,22 +9774,22 @@
         <v>54</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C55" s="47">
         <v>0</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F55" s="47">
         <v>0</v>
       </c>
       <c r="G55" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H55" s="12">
         <v>1</v>
@@ -9815,22 +9867,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C56" s="47">
         <v>0</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F56" s="47">
         <v>0</v>
       </c>
       <c r="G56" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H56" s="12">
         <v>1</v>
@@ -9908,22 +9960,22 @@
         <v>56</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C57" s="47">
         <v>0</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F57" s="47">
         <v>0</v>
       </c>
       <c r="G57" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H57" s="12">
         <v>1</v>
@@ -10001,22 +10053,22 @@
         <v>57</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C58" s="47">
         <v>0</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F58" s="47">
         <v>0</v>
       </c>
       <c r="G58" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H58" s="12">
         <v>1</v>
@@ -10094,22 +10146,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C59" s="47">
         <v>0</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F59" s="47">
         <v>0</v>
       </c>
       <c r="G59" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H59" s="12">
         <v>1</v>
@@ -10187,22 +10239,22 @@
         <v>59</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C60" s="47">
         <v>0</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F60" s="47">
         <v>0</v>
       </c>
       <c r="G60" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H60" s="12">
         <v>1</v>
@@ -10280,22 +10332,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C61" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F61" s="47">
         <v>0</v>
       </c>
       <c r="G61" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H61" s="12">
         <v>1</v>
@@ -10373,22 +10425,22 @@
         <v>61</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C62" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F62" s="47">
         <v>0</v>
       </c>
       <c r="G62" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H62" s="12">
         <v>1</v>
@@ -10466,22 +10518,22 @@
         <v>62</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C63" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F63" s="47">
         <v>0</v>
       </c>
       <c r="G63" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H63" s="12">
         <v>1</v>
@@ -10559,22 +10611,22 @@
         <v>63</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C64" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F64" s="47">
         <v>0</v>
       </c>
       <c r="G64" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H64" s="12">
         <v>1</v>
@@ -10652,22 +10704,22 @@
         <v>64</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C65" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F65" s="47">
         <v>0</v>
       </c>
       <c r="G65" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H65" s="12">
         <v>1</v>
@@ -10745,22 +10797,22 @@
         <v>65</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C66" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F66" s="47">
         <v>0</v>
       </c>
       <c r="G66" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H66" s="12">
         <v>1</v>
@@ -10838,28 +10890,28 @@
         <v>48</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C67" s="47">
         <v>0</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F67" s="47">
         <v>0</v>
       </c>
       <c r="G67" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H67" s="12">
         <v>1</v>
       </c>
       <c r="I67" s="7">
-        <f t="shared" ref="I67:I97" si="1">IF(J67=1,1,H67)</f>
+        <f t="shared" ref="I67:I98" si="1">IF(J67=1,1,H67)</f>
         <v>1</v>
       </c>
       <c r="J67" s="12">
@@ -10931,22 +10983,22 @@
         <v>49</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C68" s="59">
         <v>0</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E68" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F68" s="47">
         <v>0</v>
       </c>
       <c r="G68" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H68" s="12">
         <v>1</v>
@@ -11021,25 +11073,25 @@
     </row>
     <row r="69" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C69" s="37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F69" s="37">
         <v>0</v>
       </c>
       <c r="G69" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H69" s="22">
         <v>0</v>
@@ -11114,25 +11166,25 @@
     </row>
     <row r="70" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C70" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F70" s="38">
         <v>0</v>
       </c>
       <c r="G70" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H70" s="12">
         <v>0</v>
@@ -11207,25 +11259,25 @@
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C71" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F71" s="38">
         <v>0</v>
       </c>
       <c r="G71" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H71" s="12">
         <v>0</v>
@@ -11300,25 +11352,25 @@
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C72" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F72" s="38">
         <v>0</v>
       </c>
       <c r="G72" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H72" s="12">
         <v>0</v>
@@ -11393,25 +11445,25 @@
     </row>
     <row r="73" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C73" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F73" s="38">
         <v>0</v>
       </c>
       <c r="G73" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H73" s="12">
         <v>0</v>
@@ -11486,25 +11538,25 @@
     </row>
     <row r="74" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C74" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E74" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F74" s="38">
         <v>0</v>
       </c>
       <c r="G74" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H74" s="12">
         <v>0</v>
@@ -11579,25 +11631,25 @@
     </row>
     <row r="75" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C75" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E75" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F75" s="38">
         <v>0</v>
       </c>
       <c r="G75" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H75" s="12">
         <v>0</v>
@@ -11672,25 +11724,25 @@
     </row>
     <row r="76" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C76" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E76" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F76" s="38">
         <v>0</v>
       </c>
       <c r="G76" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H76" s="12">
         <v>0</v>
@@ -11765,25 +11817,25 @@
     </row>
     <row r="77" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C77" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E77" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F77" s="38">
         <v>0</v>
       </c>
       <c r="G77" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H77" s="12">
         <v>0</v>
@@ -11858,25 +11910,25 @@
     </row>
     <row r="78" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C78" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E78" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F78" s="38">
         <v>0</v>
       </c>
       <c r="G78" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H78" s="12">
         <v>0</v>
@@ -11951,25 +12003,25 @@
     </row>
     <row r="79" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C79" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E79" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F79" s="38">
         <v>0</v>
       </c>
       <c r="G79" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H79" s="12">
         <v>0</v>
@@ -12044,25 +12096,25 @@
     </row>
     <row r="80" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C80" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E80" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F80" s="38">
         <v>0</v>
       </c>
       <c r="G80" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H80" s="12">
         <v>0</v>
@@ -12137,25 +12189,25 @@
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C81" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E81" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F81" s="38">
         <v>0</v>
       </c>
       <c r="G81" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H81" s="12">
         <v>0</v>
@@ -12230,25 +12282,25 @@
     </row>
     <row r="82" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C82" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E82" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F82" s="38">
         <v>0</v>
       </c>
       <c r="G82" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H82" s="12">
         <v>0</v>
@@ -12323,25 +12375,25 @@
     </row>
     <row r="83" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C83" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E83" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="F83" s="38">
+        <v>0</v>
+      </c>
+      <c r="G83" s="28" t="s">
         <v>86</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="C83" s="38" t="s">
-        <v>297</v>
-      </c>
-      <c r="D83" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E83" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="F83" s="38">
-        <v>0</v>
-      </c>
-      <c r="G83" s="28" t="s">
-        <v>87</v>
       </c>
       <c r="H83" s="12">
         <v>0</v>
@@ -12416,25 +12468,25 @@
     </row>
     <row r="84" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C84" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D84" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E84" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F84" s="49">
         <v>0</v>
       </c>
       <c r="G84" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H84" s="25">
         <v>0</v>
@@ -12509,25 +12561,25 @@
     </row>
     <row r="85" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A85" s="26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C85" s="46">
         <v>0</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F85" s="46">
         <v>0</v>
       </c>
       <c r="G85" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H85" s="22">
         <v>1</v>
@@ -12602,25 +12654,25 @@
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C86" s="47">
         <v>0</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F86" s="47">
         <v>0</v>
       </c>
       <c r="G86" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H86" s="12">
         <v>1</v>
@@ -12695,25 +12747,25 @@
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C87" s="47">
         <v>0</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F87" s="47">
         <v>0</v>
       </c>
       <c r="G87" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H87" s="12">
         <v>1</v>
@@ -12788,25 +12840,25 @@
     </row>
     <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C88" s="47">
         <v>0</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F88" s="47">
         <v>0</v>
       </c>
       <c r="G88" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H88" s="12">
         <v>1</v>
@@ -12881,25 +12933,25 @@
     </row>
     <row r="89" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C89" s="47">
         <v>0</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F89" s="47">
         <v>0</v>
       </c>
       <c r="G89" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H89" s="12">
         <v>1</v>
@@ -12974,25 +13026,25 @@
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C90" s="47">
+        <v>0</v>
+      </c>
+      <c r="D90" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="B90" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="C90" s="47">
-        <v>0</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>236</v>
-      </c>
       <c r="E90" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F90" s="47">
         <v>0</v>
       </c>
       <c r="G90" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H90" s="12">
         <v>1</v>
@@ -13070,22 +13122,22 @@
         <v>67</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C91" s="37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E91" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F91" s="37">
         <v>0</v>
       </c>
       <c r="G91" s="31" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H91" s="22">
         <v>1</v>
@@ -13163,22 +13215,22 @@
         <v>68</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C92" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E92" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F92" s="38">
         <v>0</v>
       </c>
       <c r="G92" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H92" s="12">
         <v>1</v>
@@ -13252,24 +13304,26 @@
       </c>
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A93" s="10"/>
+      <c r="A93" s="10" t="s">
+        <v>310</v>
+      </c>
       <c r="B93" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C93" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E93" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F93" s="38">
         <v>0</v>
       </c>
       <c r="G93" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H93" s="12">
         <v>1</v>
@@ -13343,24 +13397,26 @@
       </c>
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A94" s="10"/>
+      <c r="A94" s="10" t="s">
+        <v>311</v>
+      </c>
       <c r="B94" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C94" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E94" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F94" s="38">
         <v>0</v>
       </c>
       <c r="G94" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H94" s="12">
         <v>1</v>
@@ -13435,25 +13491,25 @@
     </row>
     <row r="95" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>69</v>
+        <v>309</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C95" s="38">
         <v>-1</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E95" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F95" s="38">
         <v>0</v>
       </c>
       <c r="G95" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H95" s="12">
         <v>1</v>
@@ -13528,38 +13584,38 @@
     </row>
     <row r="96" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>225</v>
+        <v>312</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="C96" s="38" t="s">
-        <v>297</v>
+        <v>313</v>
+      </c>
+      <c r="C96" s="38">
+        <v>0</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>169</v>
+        <v>117</v>
       </c>
       <c r="E96" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F96" s="38">
         <v>0</v>
       </c>
       <c r="G96" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H96" s="12">
         <v>1</v>
       </c>
       <c r="I96" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I96" si="2">IF(J96=1,1,H96)</f>
         <v>1</v>
       </c>
       <c r="J96" s="12">
         <v>1</v>
       </c>
       <c r="K96" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L96" s="11">
         <v>0</v>
@@ -13592,7 +13648,7 @@
         <v>0</v>
       </c>
       <c r="V96" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W96" s="11">
         <v>0</v>
@@ -13621,25 +13677,25 @@
     </row>
     <row r="97" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C97" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>256</v>
+        <v>168</v>
+      </c>
+      <c r="E97" s="16" t="s">
+        <v>255</v>
       </c>
       <c r="F97" s="38">
         <v>0</v>
       </c>
       <c r="G97" s="28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H97" s="12">
         <v>1</v>
@@ -13712,440 +13768,549 @@
         <v>0</v>
       </c>
     </row>
+    <row r="98" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C98" s="38" t="s">
+        <v>296</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="F98" s="38">
+        <v>0</v>
+      </c>
+      <c r="G98" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="H98" s="12">
+        <v>1</v>
+      </c>
+      <c r="I98" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J98" s="12">
+        <v>1</v>
+      </c>
+      <c r="K98" s="11">
+        <v>1</v>
+      </c>
+      <c r="L98" s="11">
+        <v>0</v>
+      </c>
+      <c r="M98" s="66">
+        <v>0</v>
+      </c>
+      <c r="N98" s="15">
+        <v>0</v>
+      </c>
+      <c r="O98" s="12">
+        <v>0</v>
+      </c>
+      <c r="P98" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q98" s="11">
+        <v>0</v>
+      </c>
+      <c r="R98" s="11">
+        <v>0</v>
+      </c>
+      <c r="S98" s="11">
+        <v>0</v>
+      </c>
+      <c r="T98" s="11">
+        <v>0</v>
+      </c>
+      <c r="U98" s="11">
+        <v>0</v>
+      </c>
+      <c r="V98" s="11">
+        <v>1</v>
+      </c>
+      <c r="W98" s="11">
+        <v>0</v>
+      </c>
+      <c r="X98" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y98" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z98" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA98" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB98" s="11">
+        <v>0</v>
+      </c>
+      <c r="AC98" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD98" s="11">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J37:J40 J32:K32 J2:K11 N2:P11 J14:K14 J16:K16 O18 J17:L17 J15:L15 J12:L13 J19:L20 O21:O23 V2:V11 AD2:AD22 AA2:AB11 K95:L97 J31:L31 O29:Q30 J41:L48 J33:L36 S36:Y41 S49:X53 Z41:AD41 Z36:AD36 S12:AB22 S33:AD35 S42:AD48 S24:AB28 S32:AB32 S29:AD31 Z37:AB40 Z49:AB53 O33:Q36 O41:Q48 N31:Q31 N19:O20 N12:O17 O54:Q55 N33 N35 N37 N39 N41 N43 N45 N47 N49 N51 N53 N55 J91:K93 S54:AD97 N56:Q97 J54:L90 K94 J94:J97">
-    <cfRule type="cellIs" dxfId="209" priority="231" operator="equal">
+  <conditionalFormatting sqref="J37:J40 J32:K32 J2:K11 N2:P11 J14:K14 J16:K16 O18 J17:L17 J15:L15 J12:L13 J19:L20 O21:O23 V2:V11 AD2:AD22 AA2:AB11 K95:L95 J31:L31 O29:Q30 J41:L48 J33:L36 S36:Y41 S49:X53 Z41:AD41 Z36:AD36 S12:AB22 S33:AD35 S42:AD48 S24:AB28 S32:AB32 S29:AD31 Z37:AB40 Z49:AB53 O33:Q36 O41:Q48 N31:Q31 N19:O20 N12:O17 O54:Q55 N33 N35 N37 N39 N41 N43 N45 N47 N49 N51 N53 N55 J91:K93 S54:AD95 N56:Q95 J54:L90 K94 J94:J95 N97:Q98 S97:AD98 J97:L98">
+    <cfRule type="cellIs" dxfId="213" priority="241" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="242" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:K40 L32 L2:L11 L14 L16 L91:L94">
-    <cfRule type="cellIs" dxfId="207" priority="229" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="239" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="240" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:K18 N18">
-    <cfRule type="cellIs" dxfId="205" priority="227" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="237" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="238" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="cellIs" dxfId="203" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="235" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="236" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:K21 N21">
-    <cfRule type="cellIs" dxfId="201" priority="223" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="233" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="224" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="234" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="cellIs" dxfId="199" priority="221" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="231" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="232" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:K22 N22">
-    <cfRule type="cellIs" dxfId="197" priority="219" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="229" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="220" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="230" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="195" priority="217" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="227" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="218" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="228" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:K23 N23">
-    <cfRule type="cellIs" dxfId="193" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="225" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="226" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="cellIs" dxfId="191" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="223" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="224" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:K24 N24">
-    <cfRule type="cellIs" dxfId="189" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="221" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="222" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24">
-    <cfRule type="cellIs" dxfId="187" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="219" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="220" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25:K25 N25">
-    <cfRule type="cellIs" dxfId="185" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="217" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="218" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25">
-    <cfRule type="cellIs" dxfId="183" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="215" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="216" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:K28 N28">
-    <cfRule type="cellIs" dxfId="181" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="213" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="214" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="179" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="211" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="212" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:K29 N29">
-    <cfRule type="cellIs" dxfId="177" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="209" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="210" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L29">
-    <cfRule type="cellIs" dxfId="175" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="207" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="208" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:K30 N30 N32 N34 N36 N38 N40 N42 N44 N46 N48 N50 N52 N54">
-    <cfRule type="cellIs" dxfId="173" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="205" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="206" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="171" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="203" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="204" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L37:L40">
-    <cfRule type="cellIs" dxfId="169" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="201" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="202" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:J53">
-    <cfRule type="cellIs" dxfId="167" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="199" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="200" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:K53">
-    <cfRule type="cellIs" dxfId="165" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="197" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="198" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49:L53">
-    <cfRule type="cellIs" dxfId="163" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="195" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="196" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T23 V23 X23 AA23 AD23 P12:P23 Q13:Q22">
-    <cfRule type="cellIs" dxfId="161" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="193" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="194" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q12 U23 W23 Y23:Z23 AB23 Q23 S23">
-    <cfRule type="cellIs" dxfId="159" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="191" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="192" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q11">
-    <cfRule type="cellIs" dxfId="157" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="189" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="190" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S11">
-    <cfRule type="cellIs" dxfId="155" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="187" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="188" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z11">
-    <cfRule type="cellIs" dxfId="153" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="171" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="172" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T11">
-    <cfRule type="cellIs" dxfId="151" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="183" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="184" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U11">
-    <cfRule type="cellIs" dxfId="149" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="181" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="182" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X11">
-    <cfRule type="cellIs" dxfId="147" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="169" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="170" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W11">
-    <cfRule type="cellIs" dxfId="145" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="177" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="178" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X11">
-    <cfRule type="cellIs" dxfId="143" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="175" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="176" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P28:Q28">
-    <cfRule type="cellIs" dxfId="141" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="157" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="158" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24:Q25">
-    <cfRule type="cellIs" dxfId="139" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="161" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="162" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W11">
-    <cfRule type="cellIs" dxfId="137" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="167" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="168" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y11">
-    <cfRule type="cellIs" dxfId="135" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="165" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="166" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27:Q27">
-    <cfRule type="cellIs" dxfId="133" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="149" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="150" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P26:Q26">
-    <cfRule type="cellIs" dxfId="131" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="141" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="142" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O24:O25 AD24:AD25">
-    <cfRule type="cellIs" dxfId="129" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="163" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="164" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O28 AD28">
-    <cfRule type="cellIs" dxfId="127" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="159" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="160" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC26">
-    <cfRule type="cellIs" dxfId="125" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="129" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="130" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O26 AD26">
-    <cfRule type="cellIs" dxfId="123" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="143" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="144" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O27 AD27">
-    <cfRule type="cellIs" dxfId="121" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="151" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="152" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:K27 N26:N27">
-    <cfRule type="cellIs" dxfId="119" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="147" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="148" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26:L27">
-    <cfRule type="cellIs" dxfId="117" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="145" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="146" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC22">
-    <cfRule type="cellIs" dxfId="115" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="139" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="140" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC23">
-    <cfRule type="cellIs" dxfId="113" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="137" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="138" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC24:AC25">
-    <cfRule type="cellIs" dxfId="111" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="135" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="136" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC28">
-    <cfRule type="cellIs" dxfId="109" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="133" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="134" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC27">
-    <cfRule type="cellIs" dxfId="107" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="131" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="132" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P32:Q32">
-    <cfRule type="cellIs" dxfId="105" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="125" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="126" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC32">
-    <cfRule type="cellIs" dxfId="103" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="123" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="124" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O32 AD32">
+    <cfRule type="cellIs" dxfId="105" priority="127" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="128" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P37:Q40">
+    <cfRule type="cellIs" dxfId="103" priority="119" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="120" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC37:AC40">
     <cfRule type="cellIs" dxfId="101" priority="117" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -14153,347 +14318,371 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P37:Q40">
-    <cfRule type="cellIs" dxfId="99" priority="109" operator="equal">
+  <conditionalFormatting sqref="AD37:AD40">
+    <cfRule type="cellIs" dxfId="99" priority="121" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="110" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC37:AC40">
-    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD37:AD40">
-    <cfRule type="cellIs" dxfId="95" priority="111" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="122" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O37:O40">
-    <cfRule type="cellIs" dxfId="93" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="115" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="116" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y49:Y50">
-    <cfRule type="cellIs" dxfId="91" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="113" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="114" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P49:Q50">
-    <cfRule type="cellIs" dxfId="89" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="109" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="110" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC49:AC50">
-    <cfRule type="cellIs" dxfId="87" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="107" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="108" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD49:AD50">
-    <cfRule type="cellIs" dxfId="85" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="111" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="112" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49:O50">
-    <cfRule type="cellIs" dxfId="83" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="105" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="106" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y51:Y53">
-    <cfRule type="cellIs" dxfId="81" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="103" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="104" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P51:Q53">
-    <cfRule type="cellIs" dxfId="79" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="99" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="100" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC51:AC53">
-    <cfRule type="cellIs" dxfId="77" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="97" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="98" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD51:AD53">
-    <cfRule type="cellIs" dxfId="75" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="101" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="102" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O51:O53">
-    <cfRule type="cellIs" dxfId="73" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="95" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="96" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R12:R22 R41:R48 R24:R36 R54:R97">
-    <cfRule type="cellIs" dxfId="71" priority="83" operator="equal">
+  <conditionalFormatting sqref="R12:R22 R41:R48 R24:R36 R54:R95 R97:R98">
+    <cfRule type="cellIs" dxfId="75" priority="93" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="94" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R23">
-    <cfRule type="cellIs" dxfId="69" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="91" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="92" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R11">
-    <cfRule type="cellIs" dxfId="67" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="89" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="90" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R37:R40">
-    <cfRule type="cellIs" dxfId="65" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="87" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="88" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R49:R50">
-    <cfRule type="cellIs" dxfId="63" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="85" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="86" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R51:R53">
-    <cfRule type="cellIs" dxfId="61" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="83" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="84" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I97">
-    <cfRule type="cellIs" dxfId="59" priority="71" operator="equal">
+  <conditionalFormatting sqref="I97:I98 I2:I95">
+    <cfRule type="cellIs" dxfId="63" priority="81" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="82" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17 H19:H20 H31:H97">
-    <cfRule type="cellIs" dxfId="57" priority="47" operator="equal">
+  <conditionalFormatting sqref="H2:H17 H19:H20 H31:H95 H97:H98">
+    <cfRule type="cellIs" dxfId="61" priority="57" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="cellIs" dxfId="55" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="55" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="53" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="53" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="51" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="51" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="49" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="49" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="47" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="48" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="45" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="46" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="43" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="44" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="41" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="41" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="39" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26:H27">
-    <cfRule type="cellIs" dxfId="37" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M19:M20 M2:M17 M31:M97">
-    <cfRule type="cellIs" dxfId="35" priority="23" operator="equal">
+  <conditionalFormatting sqref="M19:M20 M2:M17 M31:M95 M97:M98">
+    <cfRule type="cellIs" dxfId="39" priority="33" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="cellIs" dxfId="33" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="31" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21">
-    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="29" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22">
-    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23">
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24">
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M25">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26:M27">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S96:AD96 N96:Q96 J96:L96">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R96">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I96">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H96">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M96">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14511,7 +14700,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14533,28 +14722,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="56" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="56" t="s">
         <v>290</v>
       </c>
-      <c r="C1" s="56" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="56" t="s">
-        <v>291</v>
-      </c>
       <c r="F1" s="56" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G1" s="56" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="I1" s="56" t="s">
         <v>266</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>267</v>
       </c>
       <c r="J1" s="56" t="s">
         <v>66</v>
@@ -14563,24 +14752,24 @@
         <v>0</v>
       </c>
       <c r="M1" s="62" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D2" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="54" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F2" s="6">
         <v>0</v>
@@ -14592,7 +14781,7 @@
         <v>26</v>
       </c>
       <c r="I2" s="54" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J2" s="21">
         <v>1</v>
@@ -14607,19 +14796,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F3" s="11">
         <v>0</v>
@@ -14631,7 +14820,7 @@
         <v>21</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J3" s="15">
         <v>1</v>
@@ -14646,19 +14835,19 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D4" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F4" s="11">
         <v>0</v>
@@ -14667,10 +14856,10 @@
         <v>26</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J4" s="15">
         <v>0</v>
@@ -14685,19 +14874,19 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D5" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F5" s="11">
         <v>0</v>
@@ -14709,7 +14898,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J5" s="15">
         <v>1</v>
@@ -14724,19 +14913,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F6" s="11">
         <v>0</v>
@@ -14748,7 +14937,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J6" s="15">
         <v>1</v>
@@ -14763,19 +14952,19 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D7" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F7" s="11">
         <v>0</v>
@@ -14802,19 +14991,19 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D8" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F8" s="11">
         <v>0</v>
@@ -14826,7 +15015,7 @@
         <v>26</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J8" s="15">
         <v>1</v>
@@ -14841,19 +15030,19 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F9" s="11">
         <v>0</v>
@@ -14865,7 +15054,7 @@
         <v>26</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J9" s="15">
         <v>1</v>
@@ -14873,19 +15062,19 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D10" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F10" s="11">
         <v>1</v>
@@ -14897,7 +15086,7 @@
         <v>21</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J10" s="15">
         <v>0</v>
@@ -14905,19 +15094,19 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D11" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F11" s="11">
         <v>1</v>
@@ -14926,10 +15115,10 @@
         <v>26</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J11" s="15">
         <v>0</v>
@@ -14937,19 +15126,19 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D12" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F12" s="11">
         <v>1</v>
@@ -14961,7 +15150,7 @@
         <v>15</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J12" s="15">
         <v>0</v>
@@ -14969,19 +15158,19 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D13" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F13" s="11">
         <v>1</v>
@@ -14993,7 +15182,7 @@
         <v>26</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J13" s="15">
         <v>0</v>
@@ -15001,19 +15190,19 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D14" s="54" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F14" s="11">
         <v>1</v>
@@ -15025,7 +15214,7 @@
         <v>16</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J14" s="15">
         <v>0</v>
@@ -15033,19 +15222,19 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F15" s="18">
         <v>0</v>
@@ -15057,7 +15246,7 @@
         <v>26</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J15" s="24">
         <v>0</v>
@@ -15065,26 +15254,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F15">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J15">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M8">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15099,7 +15288,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15109,24 +15298,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -15134,7 +15323,7 @@
         <v>66</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -15142,7 +15331,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -15150,15 +15339,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -15171,21 +15360,21 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -15193,7 +15382,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -15201,71 +15390,71 @@
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -15273,7 +15462,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -15281,7 +15470,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -15289,7 +15478,7 @@
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -15297,23 +15486,23 @@
         <v>28</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -15342,7 +15531,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -15355,7 +15544,7 @@
         <v>40</v>
       </c>
       <c r="H2" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -15401,10 +15590,10 @@
         <v>30</v>
       </c>
       <c r="H6" s="42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -15421,10 +15610,10 @@
         <v>800</v>
       </c>
       <c r="I7" s="50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -16280,7 +16469,7 @@
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="41" t="str">
         <f>cfg_var!A95</f>
-        <v>TOPOGRAPHY</v>
+        <v>TOPO_ASPECT</v>
       </c>
       <c r="B93" s="41">
         <f>cfg_var!J95*(cfg_var!K95*$H$3*(SUM(cfg_var!O95:AC95)+cfg_var!AD95*cfg_var!F95))</f>
@@ -16289,21 +16478,21 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="41" t="str">
-        <f>cfg_var!A96</f>
+        <f>cfg_var!A97</f>
         <v>U_OFLOW</v>
       </c>
       <c r="B94" s="41">
-        <f>cfg_var!J96*(cfg_var!K96*$H$3*(SUM(cfg_var!O96:AC96)+cfg_var!AD96*cfg_var!F96))</f>
+        <f>cfg_var!J97*(cfg_var!K97*$H$3*(SUM(cfg_var!O97:AC97)+cfg_var!AD97*cfg_var!F97))</f>
         <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="41" t="str">
-        <f>cfg_var!A97</f>
+        <f>cfg_var!A98</f>
         <v>V_OFLOW</v>
       </c>
       <c r="B95" s="41">
-        <f>cfg_var!J97*(cfg_var!K97*$H$3*(SUM(cfg_var!O97:AC97)+cfg_var!AD97*cfg_var!F97))</f>
+        <f>cfg_var!J98*(cfg_var!K98*$H$3*(SUM(cfg_var!O98:AC98)+cfg_var!AD98*cfg_var!F98))</f>
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed config settings for re-run 2018
</commit_message>
<xml_diff>
--- a/config/cfg_var.xlsx
+++ b/config/cfg_var.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="120" yWindow="105" windowWidth="17640" windowHeight="9525"/>
   </bookViews>
   <sheets>
-    <sheet name="cfg_var" sheetId="1" r:id="rId1"/>
+    <sheet name="cfg_var2" sheetId="1" r:id="rId1"/>
     <sheet name="combi_var" sheetId="5" r:id="rId2"/>
     <sheet name="Legend" sheetId="2" r:id="rId3"/>
     <sheet name="Input_Count" sheetId="3" r:id="rId4"/>
@@ -2289,27 +2289,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="214">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="212">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4730,8 +4710,8 @@
   <dimension ref="A1:AF98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13863,826 +13843,826 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J37:J40 J32:K32 J2:K11 N2:P11 J14:K14 J16:K16 O18 J17:L17 J15:L15 J12:L13 J19:L20 O21:O23 V2:V11 AD2:AD22 AA2:AB11 K95:L95 J31:L31 O29:Q30 J41:L48 J33:L36 S36:Y41 S49:X53 Z41:AD41 Z36:AD36 S12:AB22 S33:AD35 S42:AD48 S24:AB28 S32:AB32 S29:AD31 Z37:AB40 Z49:AB53 O33:Q36 O41:Q48 N31:Q31 N19:O20 N12:O17 O54:Q55 N33 N35 N37 N39 N41 N43 N45 N47 N49 N51 N53 N55 J91:K93 S54:AD95 N56:Q95 J54:L90 K94 J94:J95 N97:Q98 S97:AD98 J97:L98">
-    <cfRule type="cellIs" dxfId="213" priority="241" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="241" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="242" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="242" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:K40 L32 L2:L11 L14 L16 L91:L94">
-    <cfRule type="cellIs" dxfId="211" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="239" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="240" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:K18 N18">
-    <cfRule type="cellIs" dxfId="209" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="237" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="238" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="238" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="cellIs" dxfId="207" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="235" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="236" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:K21 N21">
-    <cfRule type="cellIs" dxfId="205" priority="233" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="233" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="234" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="cellIs" dxfId="203" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="231" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="232" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:K22 N22">
-    <cfRule type="cellIs" dxfId="201" priority="229" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="229" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="230" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="199" priority="227" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="227" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="228" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:K23 N23">
-    <cfRule type="cellIs" dxfId="197" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="225" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="226" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="cellIs" dxfId="195" priority="223" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="223" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="224" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="224" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:K24 N24">
-    <cfRule type="cellIs" dxfId="193" priority="221" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="221" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="222" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24">
-    <cfRule type="cellIs" dxfId="191" priority="219" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="219" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="220" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="220" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25:K25 N25">
-    <cfRule type="cellIs" dxfId="189" priority="217" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="217" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="218" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="218" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25">
-    <cfRule type="cellIs" dxfId="187" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="215" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="216" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:K28 N28">
-    <cfRule type="cellIs" dxfId="185" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="213" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="214" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="183" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="211" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="212" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:K29 N29">
-    <cfRule type="cellIs" dxfId="181" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="209" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="210" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L29">
-    <cfRule type="cellIs" dxfId="179" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="207" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="208" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:K30 N30 N32 N34 N36 N38 N40 N42 N44 N46 N48 N50 N52 N54">
-    <cfRule type="cellIs" dxfId="177" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="205" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="206" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="175" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="203" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="204" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L37:L40">
-    <cfRule type="cellIs" dxfId="173" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="201" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="202" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:J53">
-    <cfRule type="cellIs" dxfId="171" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="199" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="200" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:K53">
-    <cfRule type="cellIs" dxfId="169" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="197" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="198" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49:L53">
-    <cfRule type="cellIs" dxfId="167" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="195" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="196" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T23 V23 X23 AA23 AD23 P12:P23 Q13:Q22">
-    <cfRule type="cellIs" dxfId="165" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="193" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="194" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q12 U23 W23 Y23:Z23 AB23 Q23 S23">
-    <cfRule type="cellIs" dxfId="163" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="191" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="192" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q11">
-    <cfRule type="cellIs" dxfId="161" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="189" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="190" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S11">
-    <cfRule type="cellIs" dxfId="159" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="187" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="188" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z11">
-    <cfRule type="cellIs" dxfId="157" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="171" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="172" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T11">
-    <cfRule type="cellIs" dxfId="155" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="183" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="184" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U11">
-    <cfRule type="cellIs" dxfId="153" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="181" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="182" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X11">
-    <cfRule type="cellIs" dxfId="151" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="169" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="170" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W11">
-    <cfRule type="cellIs" dxfId="149" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="177" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="178" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X11">
-    <cfRule type="cellIs" dxfId="147" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="175" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="176" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P28:Q28">
-    <cfRule type="cellIs" dxfId="145" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="157" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="158" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24:Q25">
-    <cfRule type="cellIs" dxfId="143" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="161" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="162" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W11">
-    <cfRule type="cellIs" dxfId="141" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="167" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="168" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y11">
-    <cfRule type="cellIs" dxfId="139" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="165" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="166" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27:Q27">
-    <cfRule type="cellIs" dxfId="137" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="149" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="150" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P26:Q26">
-    <cfRule type="cellIs" dxfId="135" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="141" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="142" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O24:O25 AD24:AD25">
-    <cfRule type="cellIs" dxfId="133" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="163" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="164" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O28 AD28">
-    <cfRule type="cellIs" dxfId="131" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="159" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="160" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC26">
-    <cfRule type="cellIs" dxfId="129" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="129" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="130" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O26 AD26">
-    <cfRule type="cellIs" dxfId="127" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="143" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="144" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O27 AD27">
-    <cfRule type="cellIs" dxfId="125" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="151" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="152" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:K27 N26:N27">
-    <cfRule type="cellIs" dxfId="123" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="147" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="148" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26:L27">
-    <cfRule type="cellIs" dxfId="121" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="145" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="146" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC22">
-    <cfRule type="cellIs" dxfId="119" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="139" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="140" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC23">
-    <cfRule type="cellIs" dxfId="117" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="137" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="138" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC24:AC25">
-    <cfRule type="cellIs" dxfId="115" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="135" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="136" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC28">
-    <cfRule type="cellIs" dxfId="113" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="133" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="134" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC27">
-    <cfRule type="cellIs" dxfId="111" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="131" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="132" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P32:Q32">
-    <cfRule type="cellIs" dxfId="109" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="125" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="126" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC32">
-    <cfRule type="cellIs" dxfId="107" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="123" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="124" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O32 AD32">
-    <cfRule type="cellIs" dxfId="105" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="127" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="128" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37:Q40">
-    <cfRule type="cellIs" dxfId="103" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="119" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="120" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC37:AC40">
-    <cfRule type="cellIs" dxfId="101" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="117" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="118" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD37:AD40">
-    <cfRule type="cellIs" dxfId="99" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="121" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="122" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O37:O40">
-    <cfRule type="cellIs" dxfId="97" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="115" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="116" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y49:Y50">
-    <cfRule type="cellIs" dxfId="95" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="113" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="114" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P49:Q50">
-    <cfRule type="cellIs" dxfId="93" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="109" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="110" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC49:AC50">
-    <cfRule type="cellIs" dxfId="91" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="107" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="108" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD49:AD50">
-    <cfRule type="cellIs" dxfId="89" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="111" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="112" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49:O50">
-    <cfRule type="cellIs" dxfId="87" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="105" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="106" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y51:Y53">
-    <cfRule type="cellIs" dxfId="85" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="103" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="104" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P51:Q53">
-    <cfRule type="cellIs" dxfId="83" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="99" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="100" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC51:AC53">
-    <cfRule type="cellIs" dxfId="81" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="97" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="98" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD51:AD53">
-    <cfRule type="cellIs" dxfId="79" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="101" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="102" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O51:O53">
-    <cfRule type="cellIs" dxfId="77" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="95" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="96" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R12:R22 R41:R48 R24:R36 R54:R95 R97:R98">
-    <cfRule type="cellIs" dxfId="75" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="93" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="94" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R23">
-    <cfRule type="cellIs" dxfId="73" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="91" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="92" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R11">
-    <cfRule type="cellIs" dxfId="71" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="89" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="90" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R37:R40">
-    <cfRule type="cellIs" dxfId="69" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="87" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="88" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R49:R50">
-    <cfRule type="cellIs" dxfId="67" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="85" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="86" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R51:R53">
-    <cfRule type="cellIs" dxfId="65" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="83" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="84" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I97:I98 I2:I95">
-    <cfRule type="cellIs" dxfId="63" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="81" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="82" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H17 H19:H20 H31:H95 H97:H98">
-    <cfRule type="cellIs" dxfId="61" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="cellIs" dxfId="59" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="55" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="57" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="53" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="55" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="51" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="53" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="51" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="49" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="47" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="43" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="44" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="45" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="43" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="39" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26:H27">
-    <cfRule type="cellIs" dxfId="41" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M19:M20 M2:M17 M31:M95 M97:M98">
-    <cfRule type="cellIs" dxfId="39" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="33" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="cellIs" dxfId="37" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21">
-    <cfRule type="cellIs" dxfId="35" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="29" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22">
-    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23">
-    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24">
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M25">
-    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28">
-    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29">
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30">
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26:M27">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S96:AD96 N96:Q96 J96:L96">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R96">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I96">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H96">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M96">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15254,26 +15234,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F15">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J15">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M8">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15536,11 +15516,11 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="str">
-        <f>cfg_var!A2</f>
+        <f>cfg_var2!A2</f>
         <v>RZC</v>
       </c>
       <c r="B2" s="41">
-        <f>cfg_var!J2*(cfg_var!K2*$H$3*(SUM(cfg_var!O2:AC2)+cfg_var!AD2*cfg_var!F2))</f>
+        <f>cfg_var2!J2*(cfg_var2!K2*$H$3*(SUM(cfg_var2!O2:AC2)+cfg_var2!AD2*cfg_var2!F2))</f>
         <v>40</v>
       </c>
       <c r="H2" s="42" t="s">
@@ -15549,11 +15529,11 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="str">
-        <f>cfg_var!A3</f>
+        <f>cfg_var2!A3</f>
         <v>BZC</v>
       </c>
       <c r="B3" s="41">
-        <f>cfg_var!J3*(cfg_var!K3*$H$3*(SUM(cfg_var!O3:AC3)+cfg_var!AD3*cfg_var!F3))</f>
+        <f>cfg_var2!J3*(cfg_var2!K3*$H$3*(SUM(cfg_var2!O3:AC3)+cfg_var2!AD3*cfg_var2!F3))</f>
         <v>40</v>
       </c>
       <c r="H3" s="43">
@@ -15562,31 +15542,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="str">
-        <f>cfg_var!A4</f>
+        <f>cfg_var2!A4</f>
         <v>LZC</v>
       </c>
       <c r="B4" s="41">
-        <f>cfg_var!J4*(cfg_var!K4*$H$3*(SUM(cfg_var!O4:AC4)+cfg_var!AD4*cfg_var!F4))</f>
+        <f>cfg_var2!J4*(cfg_var2!K4*$H$3*(SUM(cfg_var2!O4:AC4)+cfg_var2!AD4*cfg_var2!F4))</f>
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="str">
-        <f>cfg_var!A5</f>
+        <f>cfg_var2!A5</f>
         <v>MZC</v>
       </c>
       <c r="B5" s="41">
-        <f>cfg_var!J5*(cfg_var!K5*$H$3*(SUM(cfg_var!O5:AC5)+cfg_var!AD5*cfg_var!F5))</f>
+        <f>cfg_var2!J5*(cfg_var2!K5*$H$3*(SUM(cfg_var2!O5:AC5)+cfg_var2!AD5*cfg_var2!F5))</f>
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="str">
-        <f>cfg_var!A6</f>
+        <f>cfg_var2!A6</f>
         <v>EZC15</v>
       </c>
       <c r="B6" s="41">
-        <f>cfg_var!J6*(cfg_var!K6*$H$3*(SUM(cfg_var!O6:AC6)+cfg_var!AD6*cfg_var!F6))</f>
+        <f>cfg_var2!J6*(cfg_var2!K6*$H$3*(SUM(cfg_var2!O6:AC6)+cfg_var2!AD6*cfg_var2!F6))</f>
         <v>30</v>
       </c>
       <c r="H6" s="42" t="s">
@@ -15598,11 +15578,11 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="str">
-        <f>cfg_var!A7</f>
+        <f>cfg_var2!A7</f>
         <v>EZC20</v>
       </c>
       <c r="B7" s="41">
-        <f>cfg_var!J7*(cfg_var!K7*$H$3*(SUM(cfg_var!O7:AC7)+cfg_var!AD7*cfg_var!F7))</f>
+        <f>cfg_var2!J7*(cfg_var2!K7*$H$3*(SUM(cfg_var2!O7:AC7)+cfg_var2!AD7*cfg_var2!F7))</f>
         <v>30</v>
       </c>
       <c r="H7" s="44">
@@ -15618,881 +15598,881 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="str">
-        <f>cfg_var!A8</f>
+        <f>cfg_var2!A8</f>
         <v>EZC45</v>
       </c>
       <c r="B8" s="41">
-        <f>cfg_var!J8*(cfg_var!K8*$H$3*(SUM(cfg_var!O8:AC8)+cfg_var!AD8*cfg_var!F8))</f>
+        <f>cfg_var2!J8*(cfg_var2!K8*$H$3*(SUM(cfg_var2!O8:AC8)+cfg_var2!AD8*cfg_var2!F8))</f>
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="str">
-        <f>cfg_var!A9</f>
+        <f>cfg_var2!A9</f>
         <v>EZC50</v>
       </c>
       <c r="B9" s="41">
-        <f>cfg_var!J9*(cfg_var!K9*$H$3*(SUM(cfg_var!O9:AC9)+cfg_var!AD9*cfg_var!F9))</f>
+        <f>cfg_var2!J9*(cfg_var2!K9*$H$3*(SUM(cfg_var2!O9:AC9)+cfg_var2!AD9*cfg_var2!F9))</f>
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="str">
-        <f>cfg_var!A10</f>
+        <f>cfg_var2!A10</f>
         <v>CZC</v>
       </c>
       <c r="B10" s="41">
-        <f>cfg_var!J10*(cfg_var!K10*$H$3*(SUM(cfg_var!O10:AC10)+cfg_var!AD10*cfg_var!F10))</f>
+        <f>cfg_var2!J10*(cfg_var2!K10*$H$3*(SUM(cfg_var2!O10:AC10)+cfg_var2!AD10*cfg_var2!F10))</f>
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="str">
-        <f>cfg_var!A11</f>
+        <f>cfg_var2!A11</f>
         <v>HZT</v>
       </c>
       <c r="B11" s="41">
-        <f>cfg_var!J11*(cfg_var!K11*$H$3*(SUM(cfg_var!O11:AC11)+cfg_var!AD11*cfg_var!F11))</f>
+        <f>cfg_var2!J11*(cfg_var2!K11*$H$3*(SUM(cfg_var2!O11:AC11)+cfg_var2!AD11*cfg_var2!F11))</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="str">
-        <f>cfg_var!A12</f>
+        <f>cfg_var2!A12</f>
         <v>IR_016</v>
       </c>
       <c r="B12" s="41">
-        <f>cfg_var!J12*(cfg_var!K12*$H$3*(SUM(cfg_var!O12:AC12)+cfg_var!AD12*cfg_var!F12))</f>
+        <f>cfg_var2!J12*(cfg_var2!K12*$H$3*(SUM(cfg_var2!O12:AC12)+cfg_var2!AD12*cfg_var2!F12))</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="str">
-        <f>cfg_var!A13</f>
+        <f>cfg_var2!A13</f>
         <v>IR_039</v>
       </c>
       <c r="B13" s="41">
-        <f>cfg_var!J13*(cfg_var!K13*$H$3*(SUM(cfg_var!O13:AC13)+cfg_var!AD13*cfg_var!F13))</f>
+        <f>cfg_var2!J13*(cfg_var2!K13*$H$3*(SUM(cfg_var2!O13:AC13)+cfg_var2!AD13*cfg_var2!F13))</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="str">
-        <f>cfg_var!A14</f>
+        <f>cfg_var2!A14</f>
         <v>IR_087</v>
       </c>
       <c r="B14" s="41">
-        <f>cfg_var!J14*(cfg_var!K14*$H$3*(SUM(cfg_var!O14:AC14)+cfg_var!AD14*cfg_var!F14))</f>
+        <f>cfg_var2!J14*(cfg_var2!K14*$H$3*(SUM(cfg_var2!O14:AC14)+cfg_var2!AD14*cfg_var2!F14))</f>
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="str">
-        <f>cfg_var!A15</f>
+        <f>cfg_var2!A15</f>
         <v>IR_097</v>
       </c>
       <c r="B15" s="41">
-        <f>cfg_var!J15*(cfg_var!K15*$H$3*(SUM(cfg_var!O15:AC15)+cfg_var!AD15*cfg_var!F15))</f>
+        <f>cfg_var2!J15*(cfg_var2!K15*$H$3*(SUM(cfg_var2!O15:AC15)+cfg_var2!AD15*cfg_var2!F15))</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="str">
-        <f>cfg_var!A16</f>
+        <f>cfg_var2!A16</f>
         <v>IR_108</v>
       </c>
       <c r="B16" s="41">
-        <f>cfg_var!J16*(cfg_var!K16*$H$3*(SUM(cfg_var!O16:AC16)+cfg_var!AD16*cfg_var!F16))</f>
+        <f>cfg_var2!J16*(cfg_var2!K16*$H$3*(SUM(cfg_var2!O16:AC16)+cfg_var2!AD16*cfg_var2!F16))</f>
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="41" t="str">
-        <f>cfg_var!A17</f>
+        <f>cfg_var2!A17</f>
         <v>IR_120</v>
       </c>
       <c r="B17" s="41">
-        <f>cfg_var!J17*(cfg_var!K17*$H$3*(SUM(cfg_var!O17:AC17)+cfg_var!AD17*cfg_var!F17))</f>
+        <f>cfg_var2!J17*(cfg_var2!K17*$H$3*(SUM(cfg_var2!O17:AC17)+cfg_var2!AD17*cfg_var2!F17))</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="41" t="str">
-        <f>cfg_var!A18</f>
+        <f>cfg_var2!A18</f>
         <v>IR_134</v>
       </c>
       <c r="B18" s="41">
-        <f>cfg_var!J18*(cfg_var!K18*$H$3*(SUM(cfg_var!O18:AC18)+cfg_var!AD18*cfg_var!F18))</f>
+        <f>cfg_var2!J18*(cfg_var2!K18*$H$3*(SUM(cfg_var2!O18:AC18)+cfg_var2!AD18*cfg_var2!F18))</f>
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="str">
-        <f>cfg_var!A19</f>
+        <f>cfg_var2!A19</f>
         <v>VIS006</v>
       </c>
       <c r="B19" s="41">
-        <f>cfg_var!J19*(cfg_var!K19*$H$3*(SUM(cfg_var!O19:AC19)+cfg_var!AD19*cfg_var!F19))</f>
+        <f>cfg_var2!J19*(cfg_var2!K19*$H$3*(SUM(cfg_var2!O19:AC19)+cfg_var2!AD19*cfg_var2!F19))</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="str">
-        <f>cfg_var!A20</f>
+        <f>cfg_var2!A20</f>
         <v>VIS008</v>
       </c>
       <c r="B20" s="41">
-        <f>cfg_var!J20*(cfg_var!K20*$H$3*(SUM(cfg_var!O20:AC20)+cfg_var!AD20*cfg_var!F20))</f>
+        <f>cfg_var2!J20*(cfg_var2!K20*$H$3*(SUM(cfg_var2!O20:AC20)+cfg_var2!AD20*cfg_var2!F20))</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="str">
-        <f>cfg_var!A21</f>
+        <f>cfg_var2!A21</f>
         <v>WV_062</v>
       </c>
       <c r="B21" s="41">
-        <f>cfg_var!J21*(cfg_var!K21*$H$3*(SUM(cfg_var!O21:AC21)+cfg_var!AD21*cfg_var!F21))</f>
+        <f>cfg_var2!J21*(cfg_var2!K21*$H$3*(SUM(cfg_var2!O21:AC21)+cfg_var2!AD21*cfg_var2!F21))</f>
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="str">
-        <f>cfg_var!A22</f>
+        <f>cfg_var2!A22</f>
         <v>WV_073</v>
       </c>
       <c r="B22" s="41">
-        <f>cfg_var!J22*(cfg_var!K22*$H$3*(SUM(cfg_var!O22:AC22)+cfg_var!AD22*cfg_var!F22))</f>
+        <f>cfg_var2!J22*(cfg_var2!K22*$H$3*(SUM(cfg_var2!O22:AC22)+cfg_var2!AD22*cfg_var2!F22))</f>
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="str">
-        <f>cfg_var!A23</f>
+        <f>cfg_var2!A23</f>
         <v>HRV</v>
       </c>
       <c r="B23" s="41">
-        <f>cfg_var!J23*(cfg_var!K23*$H$3*(SUM(cfg_var!O23:AC23)+cfg_var!AD23*cfg_var!F23))</f>
+        <f>cfg_var2!J23*(cfg_var2!K23*$H$3*(SUM(cfg_var2!O23:AC23)+cfg_var2!AD23*cfg_var2!F23))</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="str">
-        <f>cfg_var!A24</f>
+        <f>cfg_var2!A24</f>
         <v>CMA</v>
       </c>
       <c r="B24" s="41">
-        <f>cfg_var!J24*(cfg_var!K24*$H$3*(SUM(cfg_var!O24:AC24)+cfg_var!AD24*cfg_var!F24))</f>
+        <f>cfg_var2!J24*(cfg_var2!K24*$H$3*(SUM(cfg_var2!O24:AC24)+cfg_var2!AD24*cfg_var2!F24))</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="str">
-        <f>cfg_var!A25</f>
+        <f>cfg_var2!A25</f>
         <v>CT</v>
       </c>
       <c r="B25" s="41">
-        <f>cfg_var!J25*(cfg_var!K25*$H$3*(SUM(cfg_var!O25:AC25)+cfg_var!AD25*cfg_var!F25))</f>
+        <f>cfg_var2!J25*(cfg_var2!K25*$H$3*(SUM(cfg_var2!O25:AC25)+cfg_var2!AD25*cfg_var2!F25))</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="str">
-        <f>cfg_var!A26</f>
+        <f>cfg_var2!A26</f>
         <v>CTTH1</v>
       </c>
       <c r="B26" s="41">
-        <f>cfg_var!J26*(cfg_var!K26*$H$3*(SUM(cfg_var!O26:AC26)+cfg_var!AD26*cfg_var!F26))</f>
+        <f>cfg_var2!J26*(cfg_var2!K26*$H$3*(SUM(cfg_var2!O26:AC26)+cfg_var2!AD26*cfg_var2!F26))</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="str">
-        <f>cfg_var!A27</f>
+        <f>cfg_var2!A27</f>
         <v>CTTH2</v>
       </c>
       <c r="B27" s="41">
-        <f>cfg_var!J27*(cfg_var!K27*$H$3*(SUM(cfg_var!O27:AC27)+cfg_var!AD27*cfg_var!F27))</f>
+        <f>cfg_var2!J27*(cfg_var2!K27*$H$3*(SUM(cfg_var2!O27:AC27)+cfg_var2!AD27*cfg_var2!F27))</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="str">
-        <f>cfg_var!A28</f>
+        <f>cfg_var2!A28</f>
         <v>CTTH3</v>
       </c>
       <c r="B28" s="41">
-        <f>cfg_var!J28*(cfg_var!K28*$H$3*(SUM(cfg_var!O28:AC28)+cfg_var!AD28*cfg_var!F28))</f>
+        <f>cfg_var2!J28*(cfg_var2!K28*$H$3*(SUM(cfg_var2!O28:AC28)+cfg_var2!AD28*cfg_var2!F28))</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="str">
-        <f>cfg_var!A29</f>
+        <f>cfg_var2!A29</f>
         <v>lon_1</v>
       </c>
       <c r="B29" s="41">
-        <f>cfg_var!J29*(cfg_var!K29*$H$3*(SUM(cfg_var!O29:AC29)+cfg_var!AD29*cfg_var!F29))</f>
+        <f>cfg_var2!J29*(cfg_var2!K29*$H$3*(SUM(cfg_var2!O29:AC29)+cfg_var2!AD29*cfg_var2!F29))</f>
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="str">
-        <f>cfg_var!A30</f>
+        <f>cfg_var2!A30</f>
         <v>lat_1</v>
       </c>
       <c r="B30" s="41">
-        <f>cfg_var!J30*(cfg_var!K30*$H$3*(SUM(cfg_var!O30:AC30)+cfg_var!AD30*cfg_var!F30))</f>
+        <f>cfg_var2!J30*(cfg_var2!K30*$H$3*(SUM(cfg_var2!O30:AC30)+cfg_var2!AD30*cfg_var2!F30))</f>
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="str">
-        <f>cfg_var!A31</f>
+        <f>cfg_var2!A31</f>
         <v>TWATER</v>
       </c>
       <c r="B31" s="41">
-        <f>cfg_var!J31*(cfg_var!K31*$H$3*(SUM(cfg_var!O31:AC31)+cfg_var!AD31*cfg_var!F31))</f>
+        <f>cfg_var2!J31*(cfg_var2!K31*$H$3*(SUM(cfg_var2!O31:AC31)+cfg_var2!AD31*cfg_var2!F31))</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="str">
-        <f>cfg_var!A32</f>
+        <f>cfg_var2!A32</f>
         <v>tropopause_height</v>
       </c>
       <c r="B32" s="41">
-        <f>cfg_var!J32*(cfg_var!K32*$H$3*(SUM(cfg_var!O32:AC32)+cfg_var!AD32*cfg_var!F32))</f>
+        <f>cfg_var2!J32*(cfg_var2!K32*$H$3*(SUM(cfg_var2!O32:AC32)+cfg_var2!AD32*cfg_var2!F32))</f>
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="41" t="str">
-        <f>cfg_var!A33</f>
+        <f>cfg_var2!A33</f>
         <v>tropopause_temperature</v>
       </c>
       <c r="B33" s="41">
-        <f>cfg_var!J33*(cfg_var!K33*$H$3*(SUM(cfg_var!O33:AC33)+cfg_var!AD33*cfg_var!F33))</f>
+        <f>cfg_var2!J33*(cfg_var2!K33*$H$3*(SUM(cfg_var2!O33:AC33)+cfg_var2!AD33*cfg_var2!F33))</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="41" t="str">
-        <f>cfg_var!A34</f>
+        <f>cfg_var2!A34</f>
         <v>tropopause_pressure</v>
       </c>
       <c r="B34" s="41">
-        <f>cfg_var!J34*(cfg_var!K34*$H$3*(SUM(cfg_var!O34:AC34)+cfg_var!AD34*cfg_var!F34))</f>
+        <f>cfg_var2!J34*(cfg_var2!K34*$H$3*(SUM(cfg_var2!O34:AC34)+cfg_var2!AD34*cfg_var2!F34))</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="str">
-        <f>cfg_var!A35</f>
+        <f>cfg_var2!A35</f>
         <v>FF_10M</v>
       </c>
       <c r="B35" s="41">
-        <f>cfg_var!J35*(cfg_var!K35*$H$3*(SUM(cfg_var!O35:AC35)+cfg_var!AD35*cfg_var!F35))</f>
+        <f>cfg_var2!J35*(cfg_var2!K35*$H$3*(SUM(cfg_var2!O35:AC35)+cfg_var2!AD35*cfg_var2!F35))</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="str">
-        <f>cfg_var!A36</f>
+        <f>cfg_var2!A36</f>
         <v>VMAX_10M</v>
       </c>
       <c r="B36" s="41">
-        <f>cfg_var!J36*(cfg_var!K36*$H$3*(SUM(cfg_var!O36:AC36)+cfg_var!AD36*cfg_var!F36))</f>
+        <f>cfg_var2!J36*(cfg_var2!K36*$H$3*(SUM(cfg_var2!O36:AC36)+cfg_var2!AD36*cfg_var2!F36))</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="41" t="str">
-        <f>cfg_var!A37</f>
+        <f>cfg_var2!A37</f>
         <v>CAPE_MU</v>
       </c>
       <c r="B37" s="41">
-        <f>cfg_var!J37*(cfg_var!K37*$H$3*(SUM(cfg_var!O37:AC37)+cfg_var!AD37*cfg_var!F37))</f>
+        <f>cfg_var2!J37*(cfg_var2!K37*$H$3*(SUM(cfg_var2!O37:AC37)+cfg_var2!AD37*cfg_var2!F37))</f>
         <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="41" t="str">
-        <f>cfg_var!A38</f>
+        <f>cfg_var2!A38</f>
         <v>CAPE_ML</v>
       </c>
       <c r="B38" s="41">
-        <f>cfg_var!J38*(cfg_var!K38*$H$3*(SUM(cfg_var!O38:AC38)+cfg_var!AD38*cfg_var!F38))</f>
+        <f>cfg_var2!J38*(cfg_var2!K38*$H$3*(SUM(cfg_var2!O38:AC38)+cfg_var2!AD38*cfg_var2!F38))</f>
         <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="str">
-        <f>cfg_var!A39</f>
+        <f>cfg_var2!A39</f>
         <v>CIN_MU</v>
       </c>
       <c r="B39" s="41">
-        <f>cfg_var!J39*(cfg_var!K39*$H$3*(SUM(cfg_var!O39:AC39)+cfg_var!AD39*cfg_var!F39))</f>
+        <f>cfg_var2!J39*(cfg_var2!K39*$H$3*(SUM(cfg_var2!O39:AC39)+cfg_var2!AD39*cfg_var2!F39))</f>
         <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="str">
-        <f>cfg_var!A40</f>
+        <f>cfg_var2!A40</f>
         <v>CIN_ML</v>
       </c>
       <c r="B40" s="41">
-        <f>cfg_var!J40*(cfg_var!K40*$H$3*(SUM(cfg_var!O40:AC40)+cfg_var!AD40*cfg_var!F40))</f>
+        <f>cfg_var2!J40*(cfg_var2!K40*$H$3*(SUM(cfg_var2!O40:AC40)+cfg_var2!AD40*cfg_var2!F40))</f>
         <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="str">
-        <f>cfg_var!A41</f>
+        <f>cfg_var2!A41</f>
         <v>SLI</v>
       </c>
       <c r="B41" s="41">
-        <f>cfg_var!J41*(cfg_var!K41*$H$3*(SUM(cfg_var!O41:AC41)+cfg_var!AD41*cfg_var!F41))</f>
+        <f>cfg_var2!J41*(cfg_var2!K41*$H$3*(SUM(cfg_var2!O41:AC41)+cfg_var2!AD41*cfg_var2!F41))</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="str">
-        <f>cfg_var!A42</f>
+        <f>cfg_var2!A42</f>
         <v>LCL_ML</v>
       </c>
       <c r="B42" s="41">
-        <f>cfg_var!J42*(cfg_var!K42*$H$3*(SUM(cfg_var!O42:AC42)+cfg_var!AD42*cfg_var!F42))</f>
+        <f>cfg_var2!J42*(cfg_var2!K42*$H$3*(SUM(cfg_var2!O42:AC42)+cfg_var2!AD42*cfg_var2!F42))</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="str">
-        <f>cfg_var!A43</f>
+        <f>cfg_var2!A43</f>
         <v>LFC_ML</v>
       </c>
       <c r="B43" s="41">
-        <f>cfg_var!J43*(cfg_var!K43*$H$3*(SUM(cfg_var!O43:AC43)+cfg_var!AD43*cfg_var!F43))</f>
+        <f>cfg_var2!J43*(cfg_var2!K43*$H$3*(SUM(cfg_var2!O43:AC43)+cfg_var2!AD43*cfg_var2!F43))</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="str">
-        <f>cfg_var!A44</f>
+        <f>cfg_var2!A44</f>
         <v>T_SO</v>
       </c>
       <c r="B44" s="41">
-        <f>cfg_var!J44*(cfg_var!K44*$H$3*(SUM(cfg_var!O44:AC44)+cfg_var!AD44*cfg_var!F44))</f>
+        <f>cfg_var2!J44*(cfg_var2!K44*$H$3*(SUM(cfg_var2!O44:AC44)+cfg_var2!AD44*cfg_var2!F44))</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="41" t="str">
-        <f>cfg_var!A45</f>
+        <f>cfg_var2!A45</f>
         <v>T_2M</v>
       </c>
       <c r="B45" s="41">
-        <f>cfg_var!J45*(cfg_var!K45*$H$3*(SUM(cfg_var!O45:AC45)+cfg_var!AD45*cfg_var!F45))</f>
+        <f>cfg_var2!J45*(cfg_var2!K45*$H$3*(SUM(cfg_var2!O45:AC45)+cfg_var2!AD45*cfg_var2!F45))</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="str">
-        <f>cfg_var!A46</f>
+        <f>cfg_var2!A46</f>
         <v>TD_2M</v>
       </c>
       <c r="B46" s="41">
-        <f>cfg_var!J46*(cfg_var!K46*$H$3*(SUM(cfg_var!O46:AC46)+cfg_var!AD46*cfg_var!F46))</f>
+        <f>cfg_var2!J46*(cfg_var2!K46*$H$3*(SUM(cfg_var2!O46:AC46)+cfg_var2!AD46*cfg_var2!F46))</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="41" t="str">
-        <f>cfg_var!A47</f>
+        <f>cfg_var2!A47</f>
         <v>GLOB</v>
       </c>
       <c r="B47" s="41">
-        <f>cfg_var!J47*(cfg_var!K47*$H$3*(SUM(cfg_var!O47:AC47)+cfg_var!AD47*cfg_var!F47))</f>
+        <f>cfg_var2!J47*(cfg_var2!K47*$H$3*(SUM(cfg_var2!O47:AC47)+cfg_var2!AD47*cfg_var2!F47))</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="41" t="str">
-        <f>cfg_var!A48</f>
+        <f>cfg_var2!A48</f>
         <v>PS</v>
       </c>
       <c r="B48" s="41">
-        <f>cfg_var!J48*(cfg_var!K48*$H$3*(SUM(cfg_var!O48:AC48)+cfg_var!AD48*cfg_var!F48))</f>
+        <f>cfg_var2!J48*(cfg_var2!K48*$H$3*(SUM(cfg_var2!O48:AC48)+cfg_var2!AD48*cfg_var2!F48))</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="41" t="str">
-        <f>cfg_var!A49</f>
+        <f>cfg_var2!A49</f>
         <v>PMSL</v>
       </c>
       <c r="B49" s="41">
-        <f>cfg_var!J49*(cfg_var!K49*$H$3*(SUM(cfg_var!O49:AC49)+cfg_var!AD49*cfg_var!F49))</f>
+        <f>cfg_var2!J49*(cfg_var2!K49*$H$3*(SUM(cfg_var2!O49:AC49)+cfg_var2!AD49*cfg_var2!F49))</f>
         <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="str">
-        <f>cfg_var!A50</f>
+        <f>cfg_var2!A50</f>
         <v>PMSLr</v>
       </c>
       <c r="B50" s="41">
-        <f>cfg_var!J50*(cfg_var!K50*$H$3*(SUM(cfg_var!O50:AC50)+cfg_var!AD50*cfg_var!F50))</f>
+        <f>cfg_var2!J50*(cfg_var2!K50*$H$3*(SUM(cfg_var2!O50:AC50)+cfg_var2!AD50*cfg_var2!F50))</f>
         <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="41" t="str">
-        <f>cfg_var!A51</f>
+        <f>cfg_var2!A51</f>
         <v>HZEROCL</v>
       </c>
       <c r="B51" s="41">
-        <f>cfg_var!J51*(cfg_var!K51*$H$3*(SUM(cfg_var!O51:AC51)+cfg_var!AD51*cfg_var!F51))</f>
+        <f>cfg_var2!J51*(cfg_var2!K51*$H$3*(SUM(cfg_var2!O51:AC51)+cfg_var2!AD51*cfg_var2!F51))</f>
         <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="41" t="str">
-        <f>cfg_var!A52</f>
+        <f>cfg_var2!A52</f>
         <v>WSHEAR_0-3km</v>
       </c>
       <c r="B52" s="41">
-        <f>cfg_var!J52*(cfg_var!K52*$H$3*(SUM(cfg_var!O52:AC52)+cfg_var!AD52*cfg_var!F52))</f>
+        <f>cfg_var2!J52*(cfg_var2!K52*$H$3*(SUM(cfg_var2!O52:AC52)+cfg_var2!AD52*cfg_var2!F52))</f>
         <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="41" t="str">
-        <f>cfg_var!A53</f>
+        <f>cfg_var2!A53</f>
         <v>WSHEAR_0-6km</v>
       </c>
       <c r="B53" s="41">
-        <f>cfg_var!J53*(cfg_var!K53*$H$3*(SUM(cfg_var!O53:AC53)+cfg_var!AD53*cfg_var!F53))</f>
+        <f>cfg_var2!J53*(cfg_var2!K53*$H$3*(SUM(cfg_var2!O53:AC53)+cfg_var2!AD53*cfg_var2!F53))</f>
         <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="41" t="str">
-        <f>cfg_var!A54</f>
+        <f>cfg_var2!A54</f>
         <v>SYNMSG_BT_CL_IR10.8</v>
       </c>
       <c r="B54" s="41">
-        <f>cfg_var!J54*(cfg_var!K54*$H$3*(SUM(cfg_var!O54:AC54)+cfg_var!AD54*cfg_var!F54))</f>
+        <f>cfg_var2!J54*(cfg_var2!K54*$H$3*(SUM(cfg_var2!O54:AC54)+cfg_var2!AD54*cfg_var2!F54))</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="41" t="str">
-        <f>cfg_var!A55</f>
+        <f>cfg_var2!A55</f>
         <v>POT_VORTIC_30000</v>
       </c>
       <c r="B55" s="41">
-        <f>cfg_var!J55*(cfg_var!K55*$H$3*(SUM(cfg_var!O55:AC55)+cfg_var!AD55*cfg_var!F55))</f>
+        <f>cfg_var2!J55*(cfg_var2!K55*$H$3*(SUM(cfg_var2!O55:AC55)+cfg_var2!AD55*cfg_var2!F55))</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="41" t="str">
-        <f>cfg_var!A56</f>
+        <f>cfg_var2!A56</f>
         <v>POT_VORTIC_50000</v>
       </c>
       <c r="B56" s="41">
-        <f>cfg_var!J56*(cfg_var!K56*$H$3*(SUM(cfg_var!O56:AC56)+cfg_var!AD56*cfg_var!F56))</f>
+        <f>cfg_var2!J56*(cfg_var2!K56*$H$3*(SUM(cfg_var2!O56:AC56)+cfg_var2!AD56*cfg_var2!F56))</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="41" t="str">
-        <f>cfg_var!A57</f>
+        <f>cfg_var2!A57</f>
         <v>POT_VORTIC_70000</v>
       </c>
       <c r="B57" s="41">
-        <f>cfg_var!J57*(cfg_var!K57*$H$3*(SUM(cfg_var!O57:AC57)+cfg_var!AD57*cfg_var!F57))</f>
+        <f>cfg_var2!J57*(cfg_var2!K57*$H$3*(SUM(cfg_var2!O57:AC57)+cfg_var2!AD57*cfg_var2!F57))</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="41" t="str">
-        <f>cfg_var!A58</f>
+        <f>cfg_var2!A58</f>
         <v>THETAE_30000</v>
       </c>
       <c r="B58" s="41">
-        <f>cfg_var!J58*(cfg_var!K58*$H$3*(SUM(cfg_var!O58:AC58)+cfg_var!AD58*cfg_var!F58))</f>
+        <f>cfg_var2!J58*(cfg_var2!K58*$H$3*(SUM(cfg_var2!O58:AC58)+cfg_var2!AD58*cfg_var2!F58))</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="41" t="str">
-        <f>cfg_var!A59</f>
+        <f>cfg_var2!A59</f>
         <v>THETAE_50000</v>
       </c>
       <c r="B59" s="41">
-        <f>cfg_var!J59*(cfg_var!K59*$H$3*(SUM(cfg_var!O59:AC59)+cfg_var!AD59*cfg_var!F59))</f>
+        <f>cfg_var2!J59*(cfg_var2!K59*$H$3*(SUM(cfg_var2!O59:AC59)+cfg_var2!AD59*cfg_var2!F59))</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="41" t="str">
-        <f>cfg_var!A60</f>
+        <f>cfg_var2!A60</f>
         <v>THETAE_70000</v>
       </c>
       <c r="B60" s="41">
-        <f>cfg_var!J60*(cfg_var!K60*$H$3*(SUM(cfg_var!O60:AC60)+cfg_var!AD60*cfg_var!F60))</f>
+        <f>cfg_var2!J60*(cfg_var2!K60*$H$3*(SUM(cfg_var2!O60:AC60)+cfg_var2!AD60*cfg_var2!F60))</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="41" t="str">
-        <f>cfg_var!A61</f>
+        <f>cfg_var2!A61</f>
         <v>MCONV_30000</v>
       </c>
       <c r="B61" s="41">
-        <f>cfg_var!J61*(cfg_var!K61*$H$3*(SUM(cfg_var!O61:AC61)+cfg_var!AD61*cfg_var!F61))</f>
+        <f>cfg_var2!J61*(cfg_var2!K61*$H$3*(SUM(cfg_var2!O61:AC61)+cfg_var2!AD61*cfg_var2!F61))</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="41" t="str">
-        <f>cfg_var!A62</f>
+        <f>cfg_var2!A62</f>
         <v>MCONV_50000</v>
       </c>
       <c r="B62" s="41">
-        <f>cfg_var!J62*(cfg_var!K62*$H$3*(SUM(cfg_var!O62:AC62)+cfg_var!AD62*cfg_var!F62))</f>
+        <f>cfg_var2!J62*(cfg_var2!K62*$H$3*(SUM(cfg_var2!O62:AC62)+cfg_var2!AD62*cfg_var2!F62))</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="41" t="str">
-        <f>cfg_var!A63</f>
+        <f>cfg_var2!A63</f>
         <v>MCONV_70000</v>
       </c>
       <c r="B63" s="41">
-        <f>cfg_var!J63*(cfg_var!K63*$H$3*(SUM(cfg_var!O63:AC63)+cfg_var!AD63*cfg_var!F63))</f>
+        <f>cfg_var2!J63*(cfg_var2!K63*$H$3*(SUM(cfg_var2!O63:AC63)+cfg_var2!AD63*cfg_var2!F63))</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="41" t="str">
-        <f>cfg_var!A64</f>
+        <f>cfg_var2!A64</f>
         <v>geopotential_height_30000</v>
       </c>
       <c r="B64" s="41">
-        <f>cfg_var!J64*(cfg_var!K64*$H$3*(SUM(cfg_var!O64:AC64)+cfg_var!AD64*cfg_var!F64))</f>
+        <f>cfg_var2!J64*(cfg_var2!K64*$H$3*(SUM(cfg_var2!O64:AC64)+cfg_var2!AD64*cfg_var2!F64))</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="41" t="str">
-        <f>cfg_var!A65</f>
+        <f>cfg_var2!A65</f>
         <v>geopotential_height_50000</v>
       </c>
       <c r="B65" s="41">
-        <f>cfg_var!J65*(cfg_var!K65*$H$3*(SUM(cfg_var!O65:AC65)+cfg_var!AD65*cfg_var!F65))</f>
+        <f>cfg_var2!J65*(cfg_var2!K65*$H$3*(SUM(cfg_var2!O65:AC65)+cfg_var2!AD65*cfg_var2!F65))</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="41" t="str">
-        <f>cfg_var!A66</f>
+        <f>cfg_var2!A66</f>
         <v>geopotential_height_70000</v>
       </c>
       <c r="B66" s="41">
-        <f>cfg_var!J66*(cfg_var!K66*$H$3*(SUM(cfg_var!O66:AC66)+cfg_var!AD66*cfg_var!F66))</f>
+        <f>cfg_var2!J66*(cfg_var2!K66*$H$3*(SUM(cfg_var2!O66:AC66)+cfg_var2!AD66*cfg_var2!F66))</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="41" t="str">
-        <f>cfg_var!A67</f>
+        <f>cfg_var2!A67</f>
         <v>RELHUM_75000</v>
       </c>
       <c r="B67" s="41">
-        <f>cfg_var!J67*(cfg_var!K67*$H$3*(SUM(cfg_var!O67:AC67)+cfg_var!AD67*cfg_var!F67))</f>
+        <f>cfg_var2!J67*(cfg_var2!K67*$H$3*(SUM(cfg_var2!O67:AC67)+cfg_var2!AD67*cfg_var2!F67))</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="41" t="str">
-        <f>cfg_var!A68</f>
+        <f>cfg_var2!A68</f>
         <v>RELHUM_85000</v>
       </c>
       <c r="B68" s="41">
-        <f>cfg_var!J68*(cfg_var!K68*$H$3*(SUM(cfg_var!O68:AC68)+cfg_var!AD68*cfg_var!F68))</f>
+        <f>cfg_var2!J68*(cfg_var2!K68*$H$3*(SUM(cfg_var2!O68:AC68)+cfg_var2!AD68*cfg_var2!F68))</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="41" t="str">
-        <f>cfg_var!A69</f>
+        <f>cfg_var2!A69</f>
         <v>U_20000</v>
       </c>
       <c r="B69" s="41">
-        <f>cfg_var!J69*(cfg_var!K69*$H$3*(SUM(cfg_var!O69:AC69)+cfg_var!AD69*cfg_var!F69))</f>
+        <f>cfg_var2!J69*(cfg_var2!K69*$H$3*(SUM(cfg_var2!O69:AC69)+cfg_var2!AD69*cfg_var2!F69))</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="41" t="str">
-        <f>cfg_var!A70</f>
+        <f>cfg_var2!A70</f>
         <v>U_30000</v>
       </c>
       <c r="B70" s="41">
-        <f>cfg_var!J70*(cfg_var!K70*$H$3*(SUM(cfg_var!O70:AC70)+cfg_var!AD70*cfg_var!F70))</f>
+        <f>cfg_var2!J70*(cfg_var2!K70*$H$3*(SUM(cfg_var2!O70:AC70)+cfg_var2!AD70*cfg_var2!F70))</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="41" t="str">
-        <f>cfg_var!A71</f>
+        <f>cfg_var2!A71</f>
         <v>U_40000</v>
       </c>
       <c r="B71" s="41">
-        <f>cfg_var!J71*(cfg_var!K71*$H$3*(SUM(cfg_var!O71:AC71)+cfg_var!AD71*cfg_var!F71))</f>
+        <f>cfg_var2!J71*(cfg_var2!K71*$H$3*(SUM(cfg_var2!O71:AC71)+cfg_var2!AD71*cfg_var2!F71))</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="41" t="str">
-        <f>cfg_var!A72</f>
+        <f>cfg_var2!A72</f>
         <v>U_50000</v>
       </c>
       <c r="B72" s="41">
-        <f>cfg_var!J72*(cfg_var!K72*$H$3*(SUM(cfg_var!O72:AC72)+cfg_var!AD72*cfg_var!F72))</f>
+        <f>cfg_var2!J72*(cfg_var2!K72*$H$3*(SUM(cfg_var2!O72:AC72)+cfg_var2!AD72*cfg_var2!F72))</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="41" t="str">
-        <f>cfg_var!A73</f>
+        <f>cfg_var2!A73</f>
         <v>U_60000</v>
       </c>
       <c r="B73" s="41">
-        <f>cfg_var!J73*(cfg_var!K73*$H$3*(SUM(cfg_var!O73:AC73)+cfg_var!AD73*cfg_var!F73))</f>
+        <f>cfg_var2!J73*(cfg_var2!K73*$H$3*(SUM(cfg_var2!O73:AC73)+cfg_var2!AD73*cfg_var2!F73))</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="41" t="str">
-        <f>cfg_var!A74</f>
+        <f>cfg_var2!A74</f>
         <v>U_70000</v>
       </c>
       <c r="B74" s="41">
-        <f>cfg_var!J74*(cfg_var!K74*$H$3*(SUM(cfg_var!O74:AC74)+cfg_var!AD74*cfg_var!F74))</f>
+        <f>cfg_var2!J74*(cfg_var2!K74*$H$3*(SUM(cfg_var2!O74:AC74)+cfg_var2!AD74*cfg_var2!F74))</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="41" t="str">
-        <f>cfg_var!A75</f>
+        <f>cfg_var2!A75</f>
         <v>U_80000</v>
       </c>
       <c r="B75" s="41">
-        <f>cfg_var!J75*(cfg_var!K75*$H$3*(SUM(cfg_var!O75:AC75)+cfg_var!AD75*cfg_var!F75))</f>
+        <f>cfg_var2!J75*(cfg_var2!K75*$H$3*(SUM(cfg_var2!O75:AC75)+cfg_var2!AD75*cfg_var2!F75))</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="41" t="str">
-        <f>cfg_var!A76</f>
+        <f>cfg_var2!A76</f>
         <v>U_90000</v>
       </c>
       <c r="B76" s="41">
-        <f>cfg_var!J76*(cfg_var!K76*$H$3*(SUM(cfg_var!O76:AC76)+cfg_var!AD76*cfg_var!F76))</f>
+        <f>cfg_var2!J76*(cfg_var2!K76*$H$3*(SUM(cfg_var2!O76:AC76)+cfg_var2!AD76*cfg_var2!F76))</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="41" t="str">
-        <f>cfg_var!A77</f>
+        <f>cfg_var2!A77</f>
         <v>V_20000</v>
       </c>
       <c r="B77" s="41">
-        <f>cfg_var!J77*(cfg_var!K77*$H$3*(SUM(cfg_var!O77:AC77)+cfg_var!AD77*cfg_var!F77))</f>
+        <f>cfg_var2!J77*(cfg_var2!K77*$H$3*(SUM(cfg_var2!O77:AC77)+cfg_var2!AD77*cfg_var2!F77))</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="41" t="str">
-        <f>cfg_var!A78</f>
+        <f>cfg_var2!A78</f>
         <v>V_30000</v>
       </c>
       <c r="B78" s="41">
-        <f>cfg_var!J78*(cfg_var!K78*$H$3*(SUM(cfg_var!O78:AC78)+cfg_var!AD78*cfg_var!F78))</f>
+        <f>cfg_var2!J78*(cfg_var2!K78*$H$3*(SUM(cfg_var2!O78:AC78)+cfg_var2!AD78*cfg_var2!F78))</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="41" t="str">
-        <f>cfg_var!A79</f>
+        <f>cfg_var2!A79</f>
         <v>V_40000</v>
       </c>
       <c r="B79" s="41">
-        <f>cfg_var!J79*(cfg_var!K79*$H$3*(SUM(cfg_var!O79:AC79)+cfg_var!AD79*cfg_var!F79))</f>
+        <f>cfg_var2!J79*(cfg_var2!K79*$H$3*(SUM(cfg_var2!O79:AC79)+cfg_var2!AD79*cfg_var2!F79))</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="41" t="str">
-        <f>cfg_var!A80</f>
+        <f>cfg_var2!A80</f>
         <v>V_50000</v>
       </c>
       <c r="B80" s="41">
-        <f>cfg_var!J80*(cfg_var!K80*$H$3*(SUM(cfg_var!O80:AC80)+cfg_var!AD80*cfg_var!F80))</f>
+        <f>cfg_var2!J80*(cfg_var2!K80*$H$3*(SUM(cfg_var2!O80:AC80)+cfg_var2!AD80*cfg_var2!F80))</f>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="41" t="str">
-        <f>cfg_var!A81</f>
+        <f>cfg_var2!A81</f>
         <v>V_60000</v>
       </c>
       <c r="B81" s="41">
-        <f>cfg_var!J81*(cfg_var!K81*$H$3*(SUM(cfg_var!O81:AC81)+cfg_var!AD81*cfg_var!F81))</f>
+        <f>cfg_var2!J81*(cfg_var2!K81*$H$3*(SUM(cfg_var2!O81:AC81)+cfg_var2!AD81*cfg_var2!F81))</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="41" t="str">
-        <f>cfg_var!A82</f>
+        <f>cfg_var2!A82</f>
         <v>V_70000</v>
       </c>
       <c r="B82" s="41">
-        <f>cfg_var!J82*(cfg_var!K82*$H$3*(SUM(cfg_var!O82:AC82)+cfg_var!AD82*cfg_var!F82))</f>
+        <f>cfg_var2!J82*(cfg_var2!K82*$H$3*(SUM(cfg_var2!O82:AC82)+cfg_var2!AD82*cfg_var2!F82))</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="41" t="str">
-        <f>cfg_var!A83</f>
+        <f>cfg_var2!A83</f>
         <v>V_80000</v>
       </c>
       <c r="B83" s="41">
-        <f>cfg_var!J83*(cfg_var!K83*$H$3*(SUM(cfg_var!O83:AC83)+cfg_var!AD83*cfg_var!F83))</f>
+        <f>cfg_var2!J83*(cfg_var2!K83*$H$3*(SUM(cfg_var2!O83:AC83)+cfg_var2!AD83*cfg_var2!F83))</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="41" t="str">
-        <f>cfg_var!A84</f>
+        <f>cfg_var2!A84</f>
         <v>V_90000</v>
       </c>
       <c r="B84" s="41">
-        <f>cfg_var!J84*(cfg_var!K84*$H$3*(SUM(cfg_var!O84:AC84)+cfg_var!AD84*cfg_var!F84))</f>
+        <f>cfg_var2!J84*(cfg_var2!K84*$H$3*(SUM(cfg_var2!O84:AC84)+cfg_var2!AD84*cfg_var2!F84))</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="41" t="str">
-        <f>cfg_var!A85</f>
+        <f>cfg_var2!A85</f>
         <v>THX_dens</v>
       </c>
       <c r="B85" s="41">
-        <f>cfg_var!J85*(cfg_var!K85*$H$3*(SUM(cfg_var!O85:AC85)+cfg_var!AD85*cfg_var!F85))</f>
+        <f>cfg_var2!J85*(cfg_var2!K85*$H$3*(SUM(cfg_var2!O85:AC85)+cfg_var2!AD85*cfg_var2!F85))</f>
         <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="41" t="str">
-        <f>cfg_var!A86</f>
+        <f>cfg_var2!A86</f>
         <v>THX_densIC</v>
       </c>
       <c r="B86" s="41">
-        <f>cfg_var!J86*(cfg_var!K86*$H$3*(SUM(cfg_var!O86:AC86)+cfg_var!AD86*cfg_var!F86))</f>
+        <f>cfg_var2!J86*(cfg_var2!K86*$H$3*(SUM(cfg_var2!O86:AC86)+cfg_var2!AD86*cfg_var2!F86))</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="41" t="str">
-        <f>cfg_var!A87</f>
+        <f>cfg_var2!A87</f>
         <v>THX_densCG</v>
       </c>
       <c r="B87" s="41">
-        <f>cfg_var!J87*(cfg_var!K87*$H$3*(SUM(cfg_var!O87:AC87)+cfg_var!AD87*cfg_var!F87))</f>
+        <f>cfg_var2!J87*(cfg_var2!K87*$H$3*(SUM(cfg_var2!O87:AC87)+cfg_var2!AD87*cfg_var2!F87))</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="41" t="str">
-        <f>cfg_var!A88</f>
+        <f>cfg_var2!A88</f>
         <v>THX_curr_abs</v>
       </c>
       <c r="B88" s="41">
-        <f>cfg_var!J88*(cfg_var!K88*$H$3*(SUM(cfg_var!O88:AC88)+cfg_var!AD88*cfg_var!F88))</f>
+        <f>cfg_var2!J88*(cfg_var2!K88*$H$3*(SUM(cfg_var2!O88:AC88)+cfg_var2!AD88*cfg_var2!F88))</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="41" t="str">
-        <f>cfg_var!A89</f>
+        <f>cfg_var2!A89</f>
         <v>THX_curr_neg</v>
       </c>
       <c r="B89" s="41">
-        <f>cfg_var!J89*(cfg_var!K89*$H$3*(SUM(cfg_var!O89:AC89)+cfg_var!AD89*cfg_var!F89))</f>
+        <f>cfg_var2!J89*(cfg_var2!K89*$H$3*(SUM(cfg_var2!O89:AC89)+cfg_var2!AD89*cfg_var2!F89))</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="41" t="str">
-        <f>cfg_var!A90</f>
+        <f>cfg_var2!A90</f>
         <v>THX_curr_pos</v>
       </c>
       <c r="B90" s="41">
-        <f>cfg_var!J90*(cfg_var!K90*$H$3*(SUM(cfg_var!O90:AC90)+cfg_var!AD90*cfg_var!F90))</f>
+        <f>cfg_var2!J90*(cfg_var2!K90*$H$3*(SUM(cfg_var2!O90:AC90)+cfg_var2!AD90*cfg_var2!F90))</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="41" t="str">
-        <f>cfg_var!A91</f>
+        <f>cfg_var2!A91</f>
         <v>SOLAR_TIME_SIN</v>
       </c>
       <c r="B91" s="41">
-        <f>cfg_var!J91*(cfg_var!K91*$H$3*(SUM(cfg_var!O91:AC91)+cfg_var!AD91*cfg_var!F91))</f>
+        <f>cfg_var2!J91*(cfg_var2!K91*$H$3*(SUM(cfg_var2!O91:AC91)+cfg_var2!AD91*cfg_var2!F91))</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="41" t="str">
-        <f>cfg_var!A92</f>
+        <f>cfg_var2!A92</f>
         <v>SOLAR_TIME_COS</v>
       </c>
       <c r="B92" s="41">
-        <f>cfg_var!J92*(cfg_var!K92*$H$3*(SUM(cfg_var!O92:AC92)+cfg_var!AD92*cfg_var!F92))</f>
+        <f>cfg_var2!J92*(cfg_var2!K92*$H$3*(SUM(cfg_var2!O92:AC92)+cfg_var2!AD92*cfg_var2!F92))</f>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="41" t="str">
-        <f>cfg_var!A95</f>
+        <f>cfg_var2!A95</f>
         <v>TOPO_ASPECT</v>
       </c>
       <c r="B93" s="41">
-        <f>cfg_var!J95*(cfg_var!K95*$H$3*(SUM(cfg_var!O95:AC95)+cfg_var!AD95*cfg_var!F95))</f>
+        <f>cfg_var2!J95*(cfg_var2!K95*$H$3*(SUM(cfg_var2!O95:AC95)+cfg_var2!AD95*cfg_var2!F95))</f>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="41" t="str">
-        <f>cfg_var!A97</f>
+        <f>cfg_var2!A97</f>
         <v>U_OFLOW</v>
       </c>
       <c r="B94" s="41">
-        <f>cfg_var!J97*(cfg_var!K97*$H$3*(SUM(cfg_var!O97:AC97)+cfg_var!AD97*cfg_var!F97))</f>
+        <f>cfg_var2!J97*(cfg_var2!K97*$H$3*(SUM(cfg_var2!O97:AC97)+cfg_var2!AD97*cfg_var2!F97))</f>
         <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="41" t="str">
-        <f>cfg_var!A98</f>
+        <f>cfg_var2!A98</f>
         <v>V_OFLOW</v>
       </c>
       <c r="B95" s="41">
-        <f>cfg_var!J98*(cfg_var!K98*$H$3*(SUM(cfg_var!O98:AC98)+cfg_var!AD98*cfg_var!F98))</f>
+        <f>cfg_var2!J98*(cfg_var2!K98*$H$3*(SUM(cfg_var2!O98:AC98)+cfg_var2!AD98*cfg_var2!F98))</f>
         <v>10</v>
       </c>
     </row>

</xml_diff>